<commit_message>
Underground Vault 번역 갱신
</commit_message>
<xml_diff>
--- a/Data/Underground Vault - 3021706489/Underground Vault - 3021706489.xlsx
+++ b/Data/Underground Vault - 3021706489/Underground Vault - 3021706489.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SteamLibrary\steamapps\common\RimWorld\Mods\MOD KOREAN TRANSLATE\trans\Underground Vault - 3021706489\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D80C954F-6D5A-489D-B94A-E167755D855F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E856C8-5DE1-4472-8901-A2A636D8A9F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1721,7 +1721,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="680">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="690">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -3709,13 +3709,6 @@
     <t>플랫폼의 이동속도를 증가시키는 지하 금고 단말기용 업그레이드 모듈입니다.</t>
   </si>
   <si>
-    <t>저장 볼트 관리용 단말기 및 액세스 포인트입니다. 번화계 타입.\n\n볼트가 바로 아래에 있습니다. AI 코어가 지상과 볼트 사이의 사물 순간이동 프로세스를 제어합니다.\n\nAI가 단말기를 작동하려면 전원이 필요합니다. 볼트에 대한 추가 액세스 포인트를 설정하기 위해 서브 단말기를 구성할 수 있습니다. 추가 업그레이드 모듈을 설치할 수 있습니다.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">액세스 포인트를 추가하기 위한 번화계 타입의 기존 단말기에 연결된 보조 단말기. </t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>플랫폼 효율성 모듈</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -3728,30 +3721,10 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>지하 볼트 단말기용 업그레이드 모듈은 깊은 지각을 뚫어 새로운 볼트 바닥을 만들 수 있습니다.\n\n모듈을 추가할 때마다 바닥 공사 시간이 단축됩니다.</t>
-  </si>
-  <si>
-    <t>저장 효율성 모뮬</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>지하 볼트 단말기용 업그레이드 모듈로 볼트 층을 재구성하여 용량을 늘릴 수 있습니다.\n\n모듈을 추가할 때마다 업그레이드의 최대 층 레벨이 증가합니다. 각 층을 업그레이드할 때마다 용량이 2배씩 증가합니다.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">물건을 텔레포트 하여 지하 금고에 보관하는 법을 연구합니다. </t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>텔레포트 효울성 모듈</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>지하 볼트 단말기의 모듈을 업그레이드하면 텔레포트 용량이 증가합니다.\n\n모듈 개수만큼 텔레포트할 수 있는 물건의 양이 증가합니다.</t>
-  </si>
-  <si>
-    <t>아이템을 보관할 수 있는 지하 볼트 입니다. 번화계 타입.\n\n다른 볼트와 달리 지상에서 내용물에 쉽게 접근할 수 없습니다. 지상으로 물건을 직접 이동하는 텔레포트에 의존합니다.\n\n볼트 안의 물건은 주변의 위험으로부터 안전합니다. 주변의 흙으로 인해 침입자가 볼트 내부에 무엇이 있는지 알 수 없습니다.</t>
-  </si>
-  <si>
     <t>볼트에서 가져올 예정</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -3772,14 +3745,87 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>하나만 가능</t>
-  </si>
-  <si>
     <t>번화계 저장 볼트 단말기 필요</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>{0}:\n{1}\n건설 {2}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>물건을 텔레포트 하여 지하 금고에 보관하는 법을 연구합니다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>저장 볼트 관리용 단말기 및 액세스 포인트입니다. 번화계 타입.\n\n볼트가 바로 아래에 있습니다. AI 코어가 지상과 볼트 사이의 사물 순간이동 프로세스를 제어합니다.\n\nAI가 단말기를 작동하려면 전원이 필요합니다. 볼트에 대한 추가 액세스 포인트를 설정하기 위해 서브 단말기를 구성할 수 있습니다. 추가 업그레이드 모듈을 설치할 수 있습니다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>액세스 포인트를 추가하기 위한 번화계 타입의 기존 단말기에 연결된 보조 단말기.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>지하 볼트 단말기용 업그레이드 모듈은 깊은 지각을 뚫어 새로운 볼트 바닥을 만들 수 있습니다.\n\n모듈을 추가할 때마다 바닥 공사 시간이 단축됩니다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>저장 효율성 모듈</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>지하 볼트 단말기용 업그레이드 모듈로 볼트 층을 재구성하여 용량을 늘릴 수 있습니다.\n\n모듈을 추가할 때마다 업그레이드의 최대 층 레벨이 증가합니다. 각 층을 업그레이드할 때마다 용량이 2배씩 증가합니다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>지하 볼트 단말기의 모듈을 업그레이드하면 텔레포트 용량이 증가합니다.\n\n모듈 개수만큼 텔레포트할 수 있는 물건의 양이 증가합니다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이템을 보관할 수 있는 지하 볼트 입니다. 번화계 타입.\n\n다른 볼트와 달리 지상에서 내용물에 쉽게 접근할 수 없습니다. 지상으로 물건을 직접 이동하는 텔레포트에 의존합니다.\n\n볼트 안의 물건은 주변의 위험으로부터 안전합니다. 주변의 흙으로 인해 침입자가 볼트 내부에 무엇이 있는지 알 수 없습니다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>예약된 작업 삭제</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>볼트와 단말기 간 아이템 운송에 대한 예약된 작업을 지웁니다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>볼트에 저장하기</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>볼트에서 가져오기</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>볼트에 {0}개 항목 저장 예정</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>볼트에서 {0}개 항목 가져올 예정</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>볼트 확장 예정 층</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>업그레이드 예정 층</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>화장이 예약된 {0} 항목</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>볼트 안의 각 석관 당 (현재/최대):\n{0} 비어있는 경우 ({1}/{2}),\n{3} 시체가 들어있는 경우 ({4}/{5}),\n{6} 명상자가 안에 있는 시체와 관련이 있으면 (최대 {7})</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>하나만 가능</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -4152,8 +4198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="F90" sqref="F90"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="F165" sqref="F165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5679,7 +5725,7 @@
         <v>500</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>679</v>
+        <v>670</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -6410,7 +6456,7 @@
         <v>546</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>668</v>
+        <v>671</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
@@ -6444,7 +6490,7 @@
         <v>552</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>660</v>
+        <v>672</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
@@ -6478,7 +6524,7 @@
         <v>558</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>661</v>
+        <v>673</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
@@ -6495,7 +6541,7 @@
         <v>561</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
@@ -6512,7 +6558,7 @@
         <v>564</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
@@ -6529,7 +6575,7 @@
         <v>467</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
@@ -6546,7 +6592,7 @@
         <v>569</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>665</v>
+        <v>674</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
@@ -6563,7 +6609,7 @@
         <v>470</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>666</v>
+        <v>675</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
@@ -6580,7 +6626,7 @@
         <v>574</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>667</v>
+        <v>676</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.3">
@@ -6597,7 +6643,7 @@
         <v>577</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>669</v>
+        <v>663</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.3">
@@ -6614,7 +6660,7 @@
         <v>580</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>670</v>
+        <v>677</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.3">
@@ -6648,7 +6694,7 @@
         <v>586</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>671</v>
+        <v>678</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.3">
@@ -6665,7 +6711,7 @@
         <v>589</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>367</v>
+        <v>679</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.3">
@@ -6682,7 +6728,7 @@
         <v>592</v>
       </c>
       <c r="F149" s="1" t="s">
-        <v>370</v>
+        <v>680</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.3">
@@ -6699,7 +6745,7 @@
         <v>595</v>
       </c>
       <c r="F150" s="1" t="s">
-        <v>373</v>
+        <v>681</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.3">
@@ -6716,7 +6762,7 @@
         <v>598</v>
       </c>
       <c r="F151" s="1" t="s">
-        <v>304</v>
+        <v>682</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.3">
@@ -6733,7 +6779,7 @@
         <v>601</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>392</v>
+        <v>683</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.3">
@@ -6750,7 +6796,7 @@
         <v>604</v>
       </c>
       <c r="F153" s="1" t="s">
-        <v>395</v>
+        <v>684</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.3">
@@ -6767,7 +6813,7 @@
         <v>607</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>401</v>
+        <v>685</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.3">
@@ -6784,7 +6830,7 @@
         <v>610</v>
       </c>
       <c r="F155" s="1" t="s">
-        <v>407</v>
+        <v>686</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.3">
@@ -6801,7 +6847,7 @@
         <v>613</v>
       </c>
       <c r="F156" s="1" t="s">
-        <v>413</v>
+        <v>687</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.3">
@@ -6818,7 +6864,7 @@
         <v>616</v>
       </c>
       <c r="F157" s="1" t="s">
-        <v>416</v>
+        <v>688</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.3">
@@ -6835,7 +6881,7 @@
         <v>619</v>
       </c>
       <c r="F158" s="1" t="s">
-        <v>672</v>
+        <v>664</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.3">
@@ -6852,7 +6898,7 @@
         <v>622</v>
       </c>
       <c r="F159" s="1" t="s">
-        <v>673</v>
+        <v>665</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.3">
@@ -6869,7 +6915,7 @@
         <v>625</v>
       </c>
       <c r="F160" s="1" t="s">
-        <v>674</v>
+        <v>666</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.3">
@@ -6886,7 +6932,7 @@
         <v>628</v>
       </c>
       <c r="F161" s="1" t="s">
-        <v>367</v>
+        <v>679</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.3">
@@ -6903,7 +6949,7 @@
         <v>631</v>
       </c>
       <c r="F162" s="1" t="s">
-        <v>675</v>
+        <v>667</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.3">
@@ -6920,7 +6966,7 @@
         <v>634</v>
       </c>
       <c r="F163" s="1" t="s">
-        <v>676</v>
+        <v>668</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.3">
@@ -6937,7 +6983,7 @@
         <v>637</v>
       </c>
       <c r="F164" s="1" t="s">
-        <v>677</v>
+        <v>689</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.3">
@@ -6954,7 +7000,7 @@
         <v>640</v>
       </c>
       <c r="F165" s="1" t="s">
-        <v>678</v>
+        <v>669</v>
       </c>
     </row>
   </sheetData>

</xml_diff>